<commit_message>
Correccion del formato del editor 2
</commit_message>
<xml_diff>
--- a/TablaPredictivaV1.xlsx
+++ b/TablaPredictivaV1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\por_s\OneDrive\Documentos\NetBeansProjects\EditorPlanet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C29ADE-091C-4B14-8258-EE77D668C06A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A8F7CE-01C6-4794-B83D-D11248E33198}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{57810E6E-0A21-499C-91E2-287DBF5E8AC4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="378">
   <si>
     <t>$</t>
   </si>
@@ -1596,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AB6E7C-481F-445C-A027-9F2C15CEC2C1}">
   <dimension ref="A1:CN122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="BB1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CD10" sqref="CD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2688,7 +2688,9 @@
       <c r="CA9" s="7"/>
       <c r="CB9" s="7"/>
       <c r="CC9" s="7"/>
-      <c r="CD9" s="7"/>
+      <c r="CD9" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="CE9" s="7"/>
       <c r="CF9" s="7"/>
       <c r="CG9" s="7"/>
@@ -14919,12 +14921,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E8297B1F9084F346B69E2C897C07EDF5" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="02434e8a07a709289c4bff34b43edbc0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="38493f2c-75c3-4eda-bd7e-b1289f87ac22" xmlns:ns4="8d622b19-33c5-45fd-8838-b7a4bba5caad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e74bec05e75104cafe7a77ea3eaf635" ns3:_="" ns4:_="">
     <xsd:import namespace="38493f2c-75c3-4eda-bd7e-b1289f87ac22"/>
@@ -15141,6 +15137,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -15151,15 +15153,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F09F71C4-1038-47FB-A486-A3D57E27E01E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9ACBCA-23EC-4DDF-B782-DBF637EF338B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15178,6 +15171,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F09F71C4-1038-47FB-A486-A3D57E27E01E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{024B8F3A-8B0A-453D-B8D4-B07A028D6BC6}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Se agrego un temporizador, y algunas clases para el semantico
</commit_message>
<xml_diff>
--- a/TablaPredictivaV1.xlsx
+++ b/TablaPredictivaV1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\por_s\OneDrive\Documentos\NetBeansProjects\EditorPlanet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A8F7CE-01C6-4794-B83D-D11248E33198}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4AC7BCA-8B29-45FB-A051-AD322958E7CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{57810E6E-0A21-499C-91E2-287DBF5E8AC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{57810E6E-0A21-499C-91E2-287DBF5E8AC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="379">
   <si>
     <t>$</t>
   </si>
@@ -1168,6 +1168,9 @@
   </si>
   <si>
     <t>256</t>
+  </si>
+  <si>
+    <t>134</t>
   </si>
 </sst>
 </file>
@@ -1596,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AB6E7C-481F-445C-A027-9F2C15CEC2C1}">
   <dimension ref="A1:CN122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BB1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CD10" sqref="CD10"/>
+    <sheetView tabSelected="1" topLeftCell="AU55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AU67" sqref="AU67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8750,7 +8753,7 @@
         <v>198</v>
       </c>
       <c r="AU66" s="5" t="s">
-        <v>199</v>
+        <v>378</v>
       </c>
       <c r="AV66" s="5"/>
       <c r="AW66" s="5"/>
@@ -14921,6 +14924,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E8297B1F9084F346B69E2C897C07EDF5" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="02434e8a07a709289c4bff34b43edbc0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="38493f2c-75c3-4eda-bd7e-b1289f87ac22" xmlns:ns4="8d622b19-33c5-45fd-8838-b7a4bba5caad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e74bec05e75104cafe7a77ea3eaf635" ns3:_="" ns4:_="">
     <xsd:import namespace="38493f2c-75c3-4eda-bd7e-b1289f87ac22"/>
@@ -15137,12 +15146,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -15153,6 +15156,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F09F71C4-1038-47FB-A486-A3D57E27E01E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B9ACBCA-23EC-4DDF-B782-DBF637EF338B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15171,15 +15183,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F09F71C4-1038-47FB-A486-A3D57E27E01E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{024B8F3A-8B0A-453D-B8D4-B07A028D6BC6}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Cambios en la gramatifca
</commit_message>
<xml_diff>
--- a/TablaPredictivaV1.xlsx
+++ b/TablaPredictivaV1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\por_s\OneDrive\Documentos\NetBeansProjects\EditorPlanet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D30378A-F985-43F0-91C0-3FF374A78A1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12257879-D6DE-4E89-95B3-7BA2BC740901}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{57810E6E-0A21-499C-91E2-287DBF5E8AC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{57810E6E-0A21-499C-91E2-287DBF5E8AC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AB6E7C-481F-445C-A027-9F2C15CEC2C1}">
   <dimension ref="A1:CN121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN109" sqref="AN109"/>
+    <sheetView tabSelected="1" topLeftCell="BB49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BV61" sqref="BV61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16116,7 +16116,7 @@
         <v>115</v>
       </c>
       <c r="BV58" s="6">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="BW58" s="13">
         <v>116</v>
@@ -16908,7 +16908,7 @@
         <v>0</v>
       </c>
       <c r="BV61" s="6">
-        <v>0</v>
+        <v>266</v>
       </c>
       <c r="BW61" s="13">
         <v>122</v>
@@ -19545,7 +19545,7 @@
         <v>0</v>
       </c>
       <c r="BU71" s="13">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="BV71" s="6">
         <v>0</v>
@@ -22980,7 +22980,7 @@
         <v>173</v>
       </c>
       <c r="BV84" s="6">
-        <v>0</v>
+        <v>173</v>
       </c>
       <c r="BW84" s="13">
         <v>173</v>

</xml_diff>